<commit_message>
Estoy pendiente con la paginacion de la tabla
</commit_message>
<xml_diff>
--- a/mi_proyecto_web/uploads/resultados_Scoring.xlsx
+++ b/mi_proyecto_web/uploads/resultados_Scoring.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -907,6 +907,1973 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>259</v>
+      </c>
+      <c r="B7" t="n">
+        <v>32044</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>B42692731</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Zona 5 (Levante)</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Pharma Shoes Iberia, S.L. - Scholl</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I7" t="n">
+        <v>44593</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>PEDRO</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>ANTONIO</t>
+        </is>
+      </c>
+      <c r="L7" t="n">
+        <v>965279669</v>
+      </c>
+      <c r="M7" t="n">
+        <v>4</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>ILOCALIZABLE</t>
+        </is>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>965279669</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>260</v>
+      </c>
+      <c r="B8" t="n">
+        <v>32886</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>46856327Z</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Zona 4 (Centro)</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Almacenelectricidad.Com</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I8" t="n">
+        <v>44682</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>FERNANDO</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>AGUADO</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
+        <v>626280012</v>
+      </c>
+      <c r="M8" t="n">
+        <v>6</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>CONTESTADOR AUTOMATICO</t>
+        </is>
+      </c>
+      <c r="Q8" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>626280012</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>261</v>
+      </c>
+      <c r="B9" t="n">
+        <v>33316</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>B21450523</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Zona 6 (Sur)</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Enuc</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I9" t="n">
+        <v>44743</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>JUAN ANTONIO</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>RAMOS</t>
+        </is>
+      </c>
+      <c r="L9" t="n">
+        <v>603217655</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>TELEFONO ERRONEO</t>
+        </is>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>603217655</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>262</v>
+      </c>
+      <c r="B10" t="n">
+        <v>33176</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>B01759141</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Zona 5 (Levante)</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Jjprime Online</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I10" t="n">
+        <v>44743</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>ALFREDO</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>JARA ROBLES</t>
+        </is>
+      </c>
+      <c r="L10" t="n">
+        <v>693833653</v>
+      </c>
+      <c r="M10" t="n">
+        <v>3</v>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>NO CONTESTA</t>
+        </is>
+      </c>
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>693833653</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>263</v>
+      </c>
+      <c r="B11" t="n">
+        <v>40379</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>B54278825</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Zona 5 (Levante)</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>40 Grados Lenceria S.L</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I11" t="n">
+        <v>44805</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>PEDRO</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="L11" t="n">
+        <v>667670384</v>
+      </c>
+      <c r="M11" t="n">
+        <v>206</v>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>TELEFONO ERRONEO</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>ya no trabaja en esa empresa desde hace 3 años</t>
+        </is>
+      </c>
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>667670384</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>264</v>
+      </c>
+      <c r="B12" t="n">
+        <v>40811</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>52967936V</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Zona 4 (Centro)</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Hair Shop</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I12" t="n">
+        <v>44866</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>PACO</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>ESTEFANIA</t>
+        </is>
+      </c>
+      <c r="L12" t="n">
+        <v>628993428</v>
+      </c>
+      <c r="M12" t="n">
+        <v>7</v>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>NO CONTESTA</t>
+        </is>
+      </c>
+      <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>628993428</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>265</v>
+      </c>
+      <c r="B13" t="n">
+        <v>40678</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>09448362P</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Zona 7 (Televentas)</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>La Magia De Samaila</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I13" t="n">
+        <v>44866</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>DANIEL</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>RODRIGUEZ ARBAS</t>
+        </is>
+      </c>
+      <c r="L13" t="n">
+        <v>657864157</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>CIERRE DE EMPRESA</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hacen envíos a través de otra cuenta </t>
+        </is>
+      </c>
+      <c r="Q13" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>657864157</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>266</v>
+      </c>
+      <c r="B14" t="n">
+        <v>40936</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>45914711H</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Zona 7 (Televentas)</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Sara Benito Martinez</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I14" t="n">
+        <v>44896</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>SARA</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>BENITO MARTINEZ</t>
+        </is>
+      </c>
+      <c r="L14" t="n">
+        <v>605495247</v>
+      </c>
+      <c r="M14" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>CONTESTADOR AUTOMATICO</t>
+        </is>
+      </c>
+      <c r="Q14" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>605495247</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>267</v>
+      </c>
+      <c r="B15" t="n">
+        <v>41264</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>23046392R</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Zona 5 (Levante)</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Miguel Ángel Escolar Garcia</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>2023</v>
+      </c>
+      <c r="I15" t="n">
+        <v>44927</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>MIGUEL ÁNGEL</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>ESCOLAR GARCIA</t>
+        </is>
+      </c>
+      <c r="L15" t="n">
+        <v>868619351</v>
+      </c>
+      <c r="M15" t="n">
+        <v>5</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>ENCUESTA REALIZADA</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NUEVA COMERCIAL YA HABLÓ CON ELLOS Y EL CLIENTE SE LO EXPLICÓ Y NO LE RESPETA EL PRECIO Y AHORA NO LES INTERESA, SI SE LE OFRECE EL MISMO PRECIO QUE SE LE HIZO INICIALMENTE
+TELÉFONO ATENCIÓN AL CLIENTE PARA LAS EMPRESAS PERSONALIZADO, ES IMPOSIBLE TENER UNA SOLUCIÓN
+NO LE LLEGABAN AL REPARTIDOR LAS SOLICITUDES DE RECOGIDA O ESO DECÍA
+</t>
+        </is>
+      </c>
+      <c r="Q15" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>868619351</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>268</v>
+      </c>
+      <c r="B16" t="n">
+        <v>41089</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>B01724145</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Zona 3 (Noreste)</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Le Cruel</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>2023</v>
+      </c>
+      <c r="I16" t="n">
+        <v>44927</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>BELEN</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>..</t>
+        </is>
+      </c>
+      <c r="L16" t="n">
+        <v>659088673</v>
+      </c>
+      <c r="M16" t="n">
+        <v>10</v>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>ENCUESTA REALIZADA</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>TASA ALTA DE PÉRDIDAS
+LES HAN ROBADO Y DE FALLOS ES MUY ALTA
+ATENCIÓN AL CLIENTE MALISIMA LA HORA DE SOLUCIONARLO NO SE HA IMPLICADO NADIE
+LAS SUBCONTRATAS SON PÉSIMAS Y MALEDUCADOS</t>
+        </is>
+      </c>
+      <c r="Q16" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>659088673</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>269</v>
+      </c>
+      <c r="B17" t="n">
+        <v>41729</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>B05422639</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Zona 7 (Televentas)</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Land Of Nature</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>2023</v>
+      </c>
+      <c r="I17" t="n">
+        <v>44986</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>NELSON</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>GARCIA</t>
+        </is>
+      </c>
+      <c r="L17" t="n">
+        <v>951480771</v>
+      </c>
+      <c r="M17" t="n">
+        <v>5</v>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>ENCUESTA REALIZADA</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>solo ha habido una incidencia con una recogida en la que por error el repartidor marco como urgente dos paquetes y un pallet completo cuando solo eran urgentes los dos paquetes.
+Se le cobró todo como urgente y reclamaron pero nadie les ha dado ninguna solución, se le ha dicho que no hay solución 
+trabajan con ontime</t>
+        </is>
+      </c>
+      <c r="Q17" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>951480771</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>270</v>
+      </c>
+      <c r="B18" t="n">
+        <v>41068</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>B72150238</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Zona 6 (Sur)</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Iml World Car S. Xxi, S.L.</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>2023</v>
+      </c>
+      <c r="I18" t="n">
+        <v>44986</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>IML WORLD CAR S. XXI</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="L18" t="n">
+        <v>956109880</v>
+      </c>
+      <c r="M18" t="n">
+        <v>66</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>ENCUESTA REALIZADA</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>ROTURAS Y RETRASOS EN LAS ENTREGAS DE 1 SEMANA DE RETRASO</t>
+        </is>
+      </c>
+      <c r="Q18" t="n">
+        <v>0</v>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>956109880</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>271</v>
+      </c>
+      <c r="B19" t="n">
+        <v>41757</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>B95437810</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Zona 2 (Norte)</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Infobibliotecas</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>2023</v>
+      </c>
+      <c r="I19" t="n">
+        <v>44986</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>OIHANE</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>ESTEBAN</t>
+        </is>
+      </c>
+      <c r="L19" t="n">
+        <v>986090806</v>
+      </c>
+      <c r="M19" t="n">
+        <v>1</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>NO CONTESTA</t>
+        </is>
+      </c>
+      <c r="Q19" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>986090806</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>272</v>
+      </c>
+      <c r="B20" t="n">
+        <v>41824</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>B88415427</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Zona 4 (Centro)</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Casa Gusmao</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>2023</v>
+      </c>
+      <c r="I20" t="n">
+        <v>45017</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>MISAEL</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>DE GUSMAO</t>
+        </is>
+      </c>
+      <c r="L20" t="n">
+        <v>663250578</v>
+      </c>
+      <c r="M20" t="n">
+        <v>74</v>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>ENCUESTA REALIZADA</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>6 MESES HACE QUE HA RECLAMADO LAS FACTURAS DE ENTREGAS QUE NO SE HAN REALIZADO
+EL REPARTIDOR HA PUESTO UNA INCIDENCIA EN UNA ENTREGA QUE ES MENTIRA</t>
+        </is>
+      </c>
+      <c r="Q20" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>663250578</t>
+        </is>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>273</v>
+      </c>
+      <c r="B21" t="n">
+        <v>42061</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>44859654V</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Zona 5 (Levante)</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Luis Arce Miñana</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>2023</v>
+      </c>
+      <c r="I21" t="n">
+        <v>45017</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>LUIS</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>ARCE MIÑANA</t>
+        </is>
+      </c>
+      <c r="L21" t="n">
+        <v>687730832</v>
+      </c>
+      <c r="M21" t="n">
+        <v>20</v>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>ENCUESTA REALIZADA</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>HABÍA VECES QUE NO PASABAN A RECOGER 
+NO TENÍA CON QUIÉN PONERSE EN CONTACTO EN MADRID PARA CUALQUIER INCIDENCIA, ATENCIÓN DIRECTA CON NADIE PARA PODER SOLUCIONARLO
+DHL Y GLS
+UN ENVÍO A LUGO DE 3 BULTOS QUE HUBO INCIDENCIA Y LE DEVOLVIMOS 2 BULTOS TODAVÍA ESTA A LA ESPERA DE 1</t>
+        </is>
+      </c>
+      <c r="Q21" t="n">
+        <v>0</v>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>687730832</t>
+        </is>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>274</v>
+      </c>
+      <c r="B22" t="n">
+        <v>42274</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>32066340Q</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Zona 6 (Sur)</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Mia Fernandez</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>2023</v>
+      </c>
+      <c r="I22" t="n">
+        <v>45047</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>MIA</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>FERNANDEZ</t>
+        </is>
+      </c>
+      <c r="L22" t="n">
+        <v>856155110</v>
+      </c>
+      <c r="M22" t="n">
+        <v>1</v>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>CONTESTADOR AUTOMATICO</t>
+        </is>
+      </c>
+      <c r="Q22" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>856155110</t>
+        </is>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>275</v>
+      </c>
+      <c r="B23" t="n">
+        <v>42385</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>B02795961</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Zona 7 (Televentas)</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Gestion Omnicanal</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>2023</v>
+      </c>
+      <c r="I23" t="n">
+        <v>45078</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>JULIAN</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>ARANCIAL</t>
+        </is>
+      </c>
+      <c r="L23" t="n">
+        <v>621184978</v>
+      </c>
+      <c r="M23" t="n">
+        <v>24</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>NO CONTESTA</t>
+        </is>
+      </c>
+      <c r="Q23" t="n">
+        <v>0</v>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>621184978</t>
+        </is>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>276</v>
+      </c>
+      <c r="B24" t="n">
+        <v>43160</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>29488611N</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Zona 6 (Sur)</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Tienda Trucos De Magia</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>2023</v>
+      </c>
+      <c r="I24" t="n">
+        <v>45200</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>LEOPOLDO</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>RAMIREZ ALMEDIA</t>
+        </is>
+      </c>
+      <c r="L24" t="n">
+        <v>665581045</v>
+      </c>
+      <c r="M24" t="n">
+        <v>6</v>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>NO CONTESTA</t>
+        </is>
+      </c>
+      <c r="Q24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>665581045</t>
+        </is>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>278</v>
+      </c>
+      <c r="B25" t="n">
+        <v>43167</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>34866798V</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Zona 6 (Sur)</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Fruteria Los Agricultores</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>2023</v>
+      </c>
+      <c r="I25" t="n">
+        <v>45261</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>BENITA</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>ALFAR</t>
+        </is>
+      </c>
+      <c r="L25" t="n">
+        <v>618338560</v>
+      </c>
+      <c r="M25" t="n">
+        <v>2</v>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>NO INTERES</t>
+        </is>
+      </c>
+      <c r="Q25" t="n">
+        <v>0</v>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>618338560</t>
+        </is>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>279</v>
+      </c>
+      <c r="B26" t="n">
+        <v>43392</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>B16963969</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Zona 3 (Noreste)</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Solesfarma</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>2023</v>
+      </c>
+      <c r="I26" t="n">
+        <v>45261</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>JORGE</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>JIMENEZ</t>
+        </is>
+      </c>
+      <c r="L26" t="n">
+        <v>619729769</v>
+      </c>
+      <c r="M26" t="n">
+        <v>33</v>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>CONTESTADOR AUTOMATICO</t>
+        </is>
+      </c>
+      <c r="Q26" t="n">
+        <v>0</v>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>619729769</t>
+        </is>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>280</v>
+      </c>
+      <c r="B27" t="n">
+        <v>43704</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>52506242W</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Zona 7 (Televentas)</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Torolandia</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>2024</v>
+      </c>
+      <c r="I27" t="n">
+        <v>45292</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>ANDRÉS MANUEL</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>FERNÁNDEZ CONEJO</t>
+        </is>
+      </c>
+      <c r="L27" t="n">
+        <v>610771770</v>
+      </c>
+      <c r="M27" t="n">
+        <v>19</v>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>CONTESTADOR AUTOMATICO</t>
+        </is>
+      </c>
+      <c r="Q27" t="n">
+        <v>0</v>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>610771770</t>
+        </is>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>282</v>
+      </c>
+      <c r="B28" t="n">
+        <v>43596</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>B97319131</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Zona 5 (Levante)</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>General De Ediciones De Arquitectura Sl.</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>2024</v>
+      </c>
+      <c r="I28" t="n">
+        <v>45292</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>JAIME</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="L28" t="n">
+        <v>963950443</v>
+      </c>
+      <c r="M28" t="n">
+        <v>13</v>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>ENCUESTA REALIZADA</t>
+        </is>
+      </c>
+      <c r="Q28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>963950443</t>
+        </is>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>283</v>
+      </c>
+      <c r="B29" t="n">
+        <v>43780</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>E54430871</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Zona 5 (Levante)</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Turkana Fishing Cb</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>2024</v>
+      </c>
+      <c r="I29" t="n">
+        <v>45292</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>CRISTIAN</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="L29" t="n">
+        <v>966752144</v>
+      </c>
+      <c r="M29" t="n">
+        <v>2</v>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>ENCUESTA REALIZADA</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>PRECIO EN VOLUMEN MÁS CARO QUE CON LA OTRA AGENCIA DE TRANSPORTES CON LA QUE TRABAJAN AHORA</t>
+        </is>
+      </c>
+      <c r="Q29" t="n">
+        <v>0</v>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>966752144</t>
+        </is>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>284</v>
+      </c>
+      <c r="B30" t="n">
+        <v>43586</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>30803717R</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Zona 6 (Sur)</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Jesus Molina Tellez</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>2024</v>
+      </c>
+      <c r="I30" t="n">
+        <v>45292</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>JESUS</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>MOLINA TELLEZ</t>
+        </is>
+      </c>
+      <c r="L30" t="n">
+        <v>957034602</v>
+      </c>
+      <c r="M30" t="n">
+        <v>93</v>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>ENCUESTA REALIZADA</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>LOS MÓDULOS DEJARON DE FUNCIONAR POR UN ATAQUE INFORMÁTICO Y POR ELLO COPIAR Y PEGAR 30 ENVÍOS DIARIOS ES MUY COMPLICADO, DESDE FEBRERO ESTABAN CON EL PROBLEMA Y EN JUNIO COMO NO SE SOLUCIONO DESPUES DE RECLAMAR EN 2 OCASIONES, DEJARON DE REALIZAR LOS ENVÍOS CON NOSOTROS 
+EN LOS ENVÍOS NO SE REGISTRABA EL NIF Y A LA HORA DE RECLAMAR EL ENVIO NO LO PODÍAN LOCALIZAR Y SE LO COBRABAN IGUAL</t>
+        </is>
+      </c>
+      <c r="Q30" t="n">
+        <v>0</v>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>957034602</t>
+        </is>
+      </c>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>285</v>
+      </c>
+      <c r="B31" t="n">
+        <v>43978</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>76433798Z</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Zona 6 (Sur)</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Pitucas Moda</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>2024</v>
+      </c>
+      <c r="I31" t="n">
+        <v>45323</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>BEATRIZ</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>CASTILLO LOZANO</t>
+        </is>
+      </c>
+      <c r="L31" t="n">
+        <v>616685992</v>
+      </c>
+      <c r="M31" t="n">
+        <v>79</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0</v>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>616685992</t>
+        </is>
+      </c>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>286</v>
+      </c>
+      <c r="B32" t="n">
+        <v>43809</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>52792179A</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Zona 5 (Levante)</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Tintaciss</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>2024</v>
+      </c>
+      <c r="I32" t="n">
+        <v>45323</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>SERGIO</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>ALEIXANDRE GIMÉNEZ</t>
+        </is>
+      </c>
+      <c r="L32" t="n">
+        <v>964920617</v>
+      </c>
+      <c r="M32" t="n">
+        <v>17</v>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>NO CONTESTA</t>
+        </is>
+      </c>
+      <c r="Q32" t="n">
+        <v>0</v>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>964920617</t>
+        </is>
+      </c>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>287</v>
+      </c>
+      <c r="B33" t="n">
+        <v>44067</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>B24664641</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Zona 1 (Noroeste)</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Verdis Nature</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
+        <v>2024</v>
+      </c>
+      <c r="I33" t="n">
+        <v>45352</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>ROSA</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>BERMEJO MARTINEZ</t>
+        </is>
+      </c>
+      <c r="L33" t="n">
+        <v>987100123</v>
+      </c>
+      <c r="M33" t="n">
+        <v>38</v>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>ILOCALIZABLE</t>
+        </is>
+      </c>
+      <c r="Q33" t="n">
+        <v>0</v>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>987100123</t>
+        </is>
+      </c>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>288</v>
+      </c>
+      <c r="B34" t="n">
+        <v>44070</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>53790462V</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Zona 5 (Levante)</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Nexolium</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Sme</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>2024</v>
+      </c>
+      <c r="I34" t="n">
+        <v>45352</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>PEDRO</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>VIVES</t>
+        </is>
+      </c>
+      <c r="L34" t="n">
+        <v>641516106</v>
+      </c>
+      <c r="M34" t="n">
+        <v>2</v>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>CIERRE DE EMPRESA</t>
+        </is>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>EMPRESA VENDIDA</t>
+        </is>
+      </c>
+      <c r="Q34" t="n">
+        <v>0</v>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>641516106</t>
+        </is>
+      </c>
+      <c r="U34" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>